<commit_message>
Create NetLogo versions of SD models
</commit_message>
<xml_diff>
--- a/birthday.xlsx
+++ b/birthday.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewtait/Documents/projects/LearningTree/decision_analysis/load/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D53A91-3EF8-284E-8E73-120157CA27BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E3809F-9F6E-3946-9CD1-E6EA54550521}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="4140" windowWidth="30540" windowHeight="20700" xr2:uid="{CE9D2311-E939-4649-9E6E-1852DAA862CF}"/>
+    <workbookView xWindow="22360" yWindow="5000" windowWidth="30540" windowHeight="20700" xr2:uid="{CE9D2311-E939-4649-9E6E-1852DAA862CF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="birthday" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -460,7 +462,7 @@
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(1, 365)</f>
-        <v>106</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <f ca="1">COUNTIF(B$2:B$24,B2)</f>
@@ -484,7 +486,7 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B24" ca="1" si="0">RANDBETWEEN(1, 365)</f>
-        <v>142</v>
+        <v>199</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C24" ca="1" si="1">COUNTIF(B$2:B$24,B3)</f>
@@ -495,7 +497,7 @@
       </c>
       <c r="F3" s="1">
         <f>SUM(I3:I1002)/1000</f>
-        <v>0.52200000000000002</v>
+        <v>0.53</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -511,7 +513,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
@@ -521,7 +523,7 @@
         <v>2</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -530,7 +532,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>161</v>
+        <v>88</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
@@ -540,7 +542,7 @@
         <v>3</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -549,7 +551,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>290</v>
+        <v>192</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
@@ -559,7 +561,7 @@
         <v>4</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -568,7 +570,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>265</v>
+        <v>76</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
@@ -587,7 +589,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>203</v>
+        <v>247</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
@@ -597,7 +599,7 @@
         <v>6</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -606,7 +608,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>207</v>
+        <v>134</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
@@ -616,7 +618,7 @@
         <v>7</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -625,7 +627,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>162</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="1"/>
@@ -635,7 +637,7 @@
         <v>8</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -644,7 +646,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>276</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
@@ -663,7 +665,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>124</v>
+        <v>86</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
@@ -682,7 +684,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>144</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
@@ -701,7 +703,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>315</v>
+        <v>115</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
@@ -720,7 +722,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>231</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
@@ -739,7 +741,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>157</v>
+        <v>96</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
@@ -758,7 +760,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
@@ -777,7 +779,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>160</v>
+        <v>357</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
@@ -796,7 +798,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
@@ -806,7 +808,7 @@
         <v>17</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -815,7 +817,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
@@ -834,7 +836,7 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>318</v>
+        <v>130</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
@@ -844,7 +846,7 @@
         <v>19</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -853,7 +855,7 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>184</v>
+        <v>113</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
@@ -863,7 +865,7 @@
         <v>20</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -872,7 +874,7 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
@@ -882,7 +884,7 @@
         <v>21</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -891,7 +893,7 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>238</v>
+        <v>132</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
@@ -917,7 +919,7 @@
         <v>24</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -925,7 +927,7 @@
         <v>25</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -933,7 +935,7 @@
         <v>26</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -941,7 +943,7 @@
         <v>27</v>
       </c>
       <c r="I29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -949,7 +951,7 @@
         <v>28</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -957,7 +959,7 @@
         <v>29</v>
       </c>
       <c r="I31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -965,7 +967,7 @@
         <v>30</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="8:9">
@@ -973,7 +975,7 @@
         <v>31</v>
       </c>
       <c r="I33">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="8:9">
@@ -989,7 +991,7 @@
         <v>33</v>
       </c>
       <c r="I35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="8:9">
@@ -997,7 +999,7 @@
         <v>34</v>
       </c>
       <c r="I36">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="8:9">
@@ -1029,7 +1031,7 @@
         <v>38</v>
       </c>
       <c r="I40">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="8:9">
@@ -1061,7 +1063,7 @@
         <v>42</v>
       </c>
       <c r="I44">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="8:9">
@@ -1093,7 +1095,7 @@
         <v>46</v>
       </c>
       <c r="I48">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="8:9">
@@ -1101,7 +1103,7 @@
         <v>47</v>
       </c>
       <c r="I49">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="8:9">
@@ -1109,7 +1111,7 @@
         <v>48</v>
       </c>
       <c r="I50">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="8:9">
@@ -1117,7 +1119,7 @@
         <v>49</v>
       </c>
       <c r="I51">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="8:9">
@@ -1125,7 +1127,7 @@
         <v>50</v>
       </c>
       <c r="I52">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="8:9">
@@ -1141,7 +1143,7 @@
         <v>52</v>
       </c>
       <c r="I54">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="8:9">
@@ -1165,7 +1167,7 @@
         <v>55</v>
       </c>
       <c r="I57">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="8:9">
@@ -1189,7 +1191,7 @@
         <v>58</v>
       </c>
       <c r="I60">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="8:9">
@@ -1197,7 +1199,7 @@
         <v>59</v>
       </c>
       <c r="I61">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="8:9">
@@ -1221,7 +1223,7 @@
         <v>62</v>
       </c>
       <c r="I64">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="8:9">
@@ -1229,7 +1231,7 @@
         <v>63</v>
       </c>
       <c r="I65">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="8:9">
@@ -1245,7 +1247,7 @@
         <v>65</v>
       </c>
       <c r="I67">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="8:9">
@@ -1269,7 +1271,7 @@
         <v>68</v>
       </c>
       <c r="I70">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="8:9">
@@ -1277,7 +1279,7 @@
         <v>69</v>
       </c>
       <c r="I71">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="8:9">
@@ -1285,7 +1287,7 @@
         <v>70</v>
       </c>
       <c r="I72">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="8:9">
@@ -1293,7 +1295,7 @@
         <v>71</v>
       </c>
       <c r="I73">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="8:9">
@@ -1301,7 +1303,7 @@
         <v>72</v>
       </c>
       <c r="I74">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="8:9">
@@ -1309,7 +1311,7 @@
         <v>73</v>
       </c>
       <c r="I75">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="8:9">
@@ -1325,7 +1327,7 @@
         <v>75</v>
       </c>
       <c r="I77">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="8:9">
@@ -1333,7 +1335,7 @@
         <v>76</v>
       </c>
       <c r="I78">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="8:9">
@@ -1341,7 +1343,7 @@
         <v>77</v>
       </c>
       <c r="I79">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="8:9">
@@ -1349,7 +1351,7 @@
         <v>78</v>
       </c>
       <c r="I80">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="8:9">
@@ -1357,7 +1359,7 @@
         <v>79</v>
       </c>
       <c r="I81">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="8:9">
@@ -1365,7 +1367,7 @@
         <v>80</v>
       </c>
       <c r="I82">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="8:9">
@@ -1373,7 +1375,7 @@
         <v>81</v>
       </c>
       <c r="I83">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="8:9">
@@ -1381,7 +1383,7 @@
         <v>82</v>
       </c>
       <c r="I84">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="8:9">
@@ -1397,7 +1399,7 @@
         <v>84</v>
       </c>
       <c r="I86">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="8:9">
@@ -1413,7 +1415,7 @@
         <v>86</v>
       </c>
       <c r="I88">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="8:9">
@@ -1429,7 +1431,7 @@
         <v>88</v>
       </c>
       <c r="I90">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="8:9">
@@ -1445,7 +1447,7 @@
         <v>90</v>
       </c>
       <c r="I92">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="8:9">
@@ -1469,7 +1471,7 @@
         <v>93</v>
       </c>
       <c r="I95">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="8:9">
@@ -1477,7 +1479,7 @@
         <v>94</v>
       </c>
       <c r="I96">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="8:9">
@@ -1501,7 +1503,7 @@
         <v>97</v>
       </c>
       <c r="I99">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="8:9">
@@ -1509,7 +1511,7 @@
         <v>98</v>
       </c>
       <c r="I100">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="8:9">
@@ -1533,7 +1535,7 @@
         <v>101</v>
       </c>
       <c r="I103">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="8:9">
@@ -1549,7 +1551,7 @@
         <v>103</v>
       </c>
       <c r="I105">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="8:9">
@@ -1565,7 +1567,7 @@
         <v>105</v>
       </c>
       <c r="I107">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="8:9">
@@ -1581,7 +1583,7 @@
         <v>107</v>
       </c>
       <c r="I109">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="8:9">
@@ -1589,7 +1591,7 @@
         <v>108</v>
       </c>
       <c r="I110">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="8:9">
@@ -1597,7 +1599,7 @@
         <v>109</v>
       </c>
       <c r="I111">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="8:9">
@@ -1605,7 +1607,7 @@
         <v>110</v>
       </c>
       <c r="I112">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="8:9">
@@ -1621,7 +1623,7 @@
         <v>112</v>
       </c>
       <c r="I114">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="8:9">
@@ -1653,7 +1655,7 @@
         <v>116</v>
       </c>
       <c r="I118">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="8:9">
@@ -1677,7 +1679,7 @@
         <v>119</v>
       </c>
       <c r="I121">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="8:9">
@@ -1685,7 +1687,7 @@
         <v>120</v>
       </c>
       <c r="I122">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="8:9">
@@ -1693,7 +1695,7 @@
         <v>121</v>
       </c>
       <c r="I123">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="8:9">
@@ -1701,7 +1703,7 @@
         <v>122</v>
       </c>
       <c r="I124">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="8:9">
@@ -1709,7 +1711,7 @@
         <v>123</v>
       </c>
       <c r="I125">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="8:9">
@@ -1725,7 +1727,7 @@
         <v>125</v>
       </c>
       <c r="I127">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="8:9">
@@ -1741,7 +1743,7 @@
         <v>127</v>
       </c>
       <c r="I129">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="8:9">
@@ -1773,7 +1775,7 @@
         <v>131</v>
       </c>
       <c r="I133">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="8:9">
@@ -1797,7 +1799,7 @@
         <v>134</v>
       </c>
       <c r="I136">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="8:9">
@@ -1861,7 +1863,7 @@
         <v>142</v>
       </c>
       <c r="I144">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="8:9">
@@ -1869,7 +1871,7 @@
         <v>143</v>
       </c>
       <c r="I145">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="8:9">
@@ -1877,7 +1879,7 @@
         <v>144</v>
       </c>
       <c r="I146">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="8:9">
@@ -1885,7 +1887,7 @@
         <v>145</v>
       </c>
       <c r="I147">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="8:9">
@@ -1893,7 +1895,7 @@
         <v>146</v>
       </c>
       <c r="I148">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="8:9">
@@ -1909,7 +1911,7 @@
         <v>148</v>
       </c>
       <c r="I150">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="8:9">
@@ -1917,7 +1919,7 @@
         <v>149</v>
       </c>
       <c r="I151">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="8:9">
@@ -1925,7 +1927,7 @@
         <v>150</v>
       </c>
       <c r="I152">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="8:9">
@@ -1941,7 +1943,7 @@
         <v>152</v>
       </c>
       <c r="I154">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="8:9">
@@ -1965,7 +1967,7 @@
         <v>155</v>
       </c>
       <c r="I157">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="8:9">
@@ -1973,7 +1975,7 @@
         <v>156</v>
       </c>
       <c r="I158">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="8:9">
@@ -1989,7 +1991,7 @@
         <v>158</v>
       </c>
       <c r="I160">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="8:9">
@@ -1997,7 +1999,7 @@
         <v>159</v>
       </c>
       <c r="I161">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162" spans="8:9">
@@ -2005,7 +2007,7 @@
         <v>160</v>
       </c>
       <c r="I162">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163" spans="8:9">
@@ -2013,7 +2015,7 @@
         <v>161</v>
       </c>
       <c r="I163">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164" spans="8:9">
@@ -2029,7 +2031,7 @@
         <v>163</v>
       </c>
       <c r="I165">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166" spans="8:9">
@@ -2053,7 +2055,7 @@
         <v>166</v>
       </c>
       <c r="I168">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169" spans="8:9">
@@ -2061,7 +2063,7 @@
         <v>167</v>
       </c>
       <c r="I169">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="8:9">
@@ -2069,7 +2071,7 @@
         <v>168</v>
       </c>
       <c r="I170">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171" spans="8:9">
@@ -2085,7 +2087,7 @@
         <v>170</v>
       </c>
       <c r="I172">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173" spans="8:9">
@@ -2093,7 +2095,7 @@
         <v>171</v>
       </c>
       <c r="I173">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="8:9">
@@ -2117,7 +2119,7 @@
         <v>174</v>
       </c>
       <c r="I176">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177" spans="8:9">
@@ -2125,7 +2127,7 @@
         <v>175</v>
       </c>
       <c r="I177">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="178" spans="8:9">
@@ -2141,7 +2143,7 @@
         <v>177</v>
       </c>
       <c r="I179">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="180" spans="8:9">
@@ -2173,7 +2175,7 @@
         <v>181</v>
       </c>
       <c r="I183">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="184" spans="8:9">
@@ -2189,7 +2191,7 @@
         <v>183</v>
       </c>
       <c r="I185">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="186" spans="8:9">
@@ -2205,7 +2207,7 @@
         <v>185</v>
       </c>
       <c r="I187">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="188" spans="8:9">
@@ -2229,7 +2231,7 @@
         <v>188</v>
       </c>
       <c r="I190">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191" spans="8:9">
@@ -2253,7 +2255,7 @@
         <v>191</v>
       </c>
       <c r="I193">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194" spans="8:9">
@@ -2261,7 +2263,7 @@
         <v>192</v>
       </c>
       <c r="I194">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195" spans="8:9">
@@ -2277,7 +2279,7 @@
         <v>194</v>
       </c>
       <c r="I196">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="197" spans="8:9">
@@ -2285,7 +2287,7 @@
         <v>195</v>
       </c>
       <c r="I197">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="198" spans="8:9">
@@ -2301,7 +2303,7 @@
         <v>197</v>
       </c>
       <c r="I199">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200" spans="8:9">
@@ -2309,7 +2311,7 @@
         <v>198</v>
       </c>
       <c r="I200">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="201" spans="8:9">
@@ -2325,7 +2327,7 @@
         <v>200</v>
       </c>
       <c r="I202">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="203" spans="8:9">
@@ -2333,7 +2335,7 @@
         <v>201</v>
       </c>
       <c r="I203">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204" spans="8:9">
@@ -2357,7 +2359,7 @@
         <v>204</v>
       </c>
       <c r="I206">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="207" spans="8:9">
@@ -2373,7 +2375,7 @@
         <v>206</v>
       </c>
       <c r="I208">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="209" spans="8:9">
@@ -2381,7 +2383,7 @@
         <v>207</v>
       </c>
       <c r="I209">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="210" spans="8:9">
@@ -2397,7 +2399,7 @@
         <v>209</v>
       </c>
       <c r="I211">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="212" spans="8:9">
@@ -2405,7 +2407,7 @@
         <v>210</v>
       </c>
       <c r="I212">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="213" spans="8:9">
@@ -2413,7 +2415,7 @@
         <v>211</v>
       </c>
       <c r="I213">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="214" spans="8:9">
@@ -2421,7 +2423,7 @@
         <v>212</v>
       </c>
       <c r="I214">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="215" spans="8:9">
@@ -2429,7 +2431,7 @@
         <v>213</v>
       </c>
       <c r="I215">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="216" spans="8:9">
@@ -2461,7 +2463,7 @@
         <v>217</v>
       </c>
       <c r="I219">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="220" spans="8:9">
@@ -2469,7 +2471,7 @@
         <v>218</v>
       </c>
       <c r="I220">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="221" spans="8:9">
@@ -2477,7 +2479,7 @@
         <v>219</v>
       </c>
       <c r="I221">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="222" spans="8:9">
@@ -2517,7 +2519,7 @@
         <v>224</v>
       </c>
       <c r="I226">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="227" spans="8:9">
@@ -2525,7 +2527,7 @@
         <v>225</v>
       </c>
       <c r="I227">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="228" spans="8:9">
@@ -2533,7 +2535,7 @@
         <v>226</v>
       </c>
       <c r="I228">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="229" spans="8:9">
@@ -2541,7 +2543,7 @@
         <v>227</v>
       </c>
       <c r="I229">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="230" spans="8:9">
@@ -2549,7 +2551,7 @@
         <v>228</v>
       </c>
       <c r="I230">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="231" spans="8:9">
@@ -2565,7 +2567,7 @@
         <v>230</v>
       </c>
       <c r="I232">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="233" spans="8:9">
@@ -2581,7 +2583,7 @@
         <v>232</v>
       </c>
       <c r="I234">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="235" spans="8:9">
@@ -2621,7 +2623,7 @@
         <v>237</v>
       </c>
       <c r="I239">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="240" spans="8:9">
@@ -2629,7 +2631,7 @@
         <v>238</v>
       </c>
       <c r="I240">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="241" spans="8:9">
@@ -2653,7 +2655,7 @@
         <v>241</v>
       </c>
       <c r="I243">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="244" spans="8:9">
@@ -2661,7 +2663,7 @@
         <v>242</v>
       </c>
       <c r="I244">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="245" spans="8:9">
@@ -2685,7 +2687,7 @@
         <v>245</v>
       </c>
       <c r="I247">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="248" spans="8:9">
@@ -2693,7 +2695,7 @@
         <v>246</v>
       </c>
       <c r="I248">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="249" spans="8:9">
@@ -2701,7 +2703,7 @@
         <v>247</v>
       </c>
       <c r="I249">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="250" spans="8:9">
@@ -2709,7 +2711,7 @@
         <v>248</v>
       </c>
       <c r="I250">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="251" spans="8:9">
@@ -2725,7 +2727,7 @@
         <v>250</v>
       </c>
       <c r="I252">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="253" spans="8:9">
@@ -2733,7 +2735,7 @@
         <v>251</v>
       </c>
       <c r="I253">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="254" spans="8:9">
@@ -2749,7 +2751,7 @@
         <v>253</v>
       </c>
       <c r="I255">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="256" spans="8:9">
@@ -2757,7 +2759,7 @@
         <v>254</v>
       </c>
       <c r="I256">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="257" spans="8:9">
@@ -2789,7 +2791,7 @@
         <v>258</v>
       </c>
       <c r="I260">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="261" spans="8:9">
@@ -2797,7 +2799,7 @@
         <v>259</v>
       </c>
       <c r="I261">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="262" spans="8:9">
@@ -2805,7 +2807,7 @@
         <v>260</v>
       </c>
       <c r="I262">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="263" spans="8:9">
@@ -2829,7 +2831,7 @@
         <v>263</v>
       </c>
       <c r="I265">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="266" spans="8:9">
@@ -2869,7 +2871,7 @@
         <v>268</v>
       </c>
       <c r="I270">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="271" spans="8:9">
@@ -2885,7 +2887,7 @@
         <v>270</v>
       </c>
       <c r="I272">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="273" spans="8:9">
@@ -2957,7 +2959,7 @@
         <v>279</v>
       </c>
       <c r="I281">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="282" spans="8:9">
@@ -2965,7 +2967,7 @@
         <v>280</v>
       </c>
       <c r="I282">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="283" spans="8:9">
@@ -2973,7 +2975,7 @@
         <v>281</v>
       </c>
       <c r="I283">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="284" spans="8:9">
@@ -2981,7 +2983,7 @@
         <v>282</v>
       </c>
       <c r="I284">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="285" spans="8:9">
@@ -2989,7 +2991,7 @@
         <v>283</v>
       </c>
       <c r="I285">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="286" spans="8:9">
@@ -3005,7 +3007,7 @@
         <v>285</v>
       </c>
       <c r="I287">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="288" spans="8:9">
@@ -3021,7 +3023,7 @@
         <v>287</v>
       </c>
       <c r="I289">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="290" spans="8:9">
@@ -3069,7 +3071,7 @@
         <v>293</v>
       </c>
       <c r="I295">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="296" spans="8:9">
@@ -3077,7 +3079,7 @@
         <v>294</v>
       </c>
       <c r="I296">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="297" spans="8:9">
@@ -3085,7 +3087,7 @@
         <v>295</v>
       </c>
       <c r="I297">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="298" spans="8:9">
@@ -3093,7 +3095,7 @@
         <v>296</v>
       </c>
       <c r="I298">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="299" spans="8:9">
@@ -3101,7 +3103,7 @@
         <v>297</v>
       </c>
       <c r="I299">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="300" spans="8:9">
@@ -3117,7 +3119,7 @@
         <v>299</v>
       </c>
       <c r="I301">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="302" spans="8:9">
@@ -3165,7 +3167,7 @@
         <v>305</v>
       </c>
       <c r="I307">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="308" spans="8:9">
@@ -3173,7 +3175,7 @@
         <v>306</v>
       </c>
       <c r="I308">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="309" spans="8:9">
@@ -3189,7 +3191,7 @@
         <v>308</v>
       </c>
       <c r="I310">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="311" spans="8:9">
@@ -3197,7 +3199,7 @@
         <v>309</v>
       </c>
       <c r="I311">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="312" spans="8:9">
@@ -3213,7 +3215,7 @@
         <v>311</v>
       </c>
       <c r="I313">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="314" spans="8:9">
@@ -3229,7 +3231,7 @@
         <v>313</v>
       </c>
       <c r="I315">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="316" spans="8:9">
@@ -3253,7 +3255,7 @@
         <v>316</v>
       </c>
       <c r="I318">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="319" spans="8:9">
@@ -3293,7 +3295,7 @@
         <v>321</v>
       </c>
       <c r="I323">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="324" spans="8:9">
@@ -3309,7 +3311,7 @@
         <v>323</v>
       </c>
       <c r="I325">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="326" spans="8:9">
@@ -3325,7 +3327,7 @@
         <v>325</v>
       </c>
       <c r="I327">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="328" spans="8:9">
@@ -3333,7 +3335,7 @@
         <v>326</v>
       </c>
       <c r="I328">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="329" spans="8:9">
@@ -3365,7 +3367,7 @@
         <v>330</v>
       </c>
       <c r="I332">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="333" spans="8:9">
@@ -3405,7 +3407,7 @@
         <v>335</v>
       </c>
       <c r="I337">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="338" spans="8:9">
@@ -3429,7 +3431,7 @@
         <v>338</v>
       </c>
       <c r="I340">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="341" spans="8:9">
@@ -3445,7 +3447,7 @@
         <v>340</v>
       </c>
       <c r="I342">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="343" spans="8:9">
@@ -3453,7 +3455,7 @@
         <v>341</v>
       </c>
       <c r="I343">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="344" spans="8:9">
@@ -3477,7 +3479,7 @@
         <v>344</v>
       </c>
       <c r="I346">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="347" spans="8:9">
@@ -3493,7 +3495,7 @@
         <v>346</v>
       </c>
       <c r="I348">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="349" spans="8:9">
@@ -3509,7 +3511,7 @@
         <v>348</v>
       </c>
       <c r="I350">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="351" spans="8:9">
@@ -3517,7 +3519,7 @@
         <v>349</v>
       </c>
       <c r="I351">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="352" spans="8:9">
@@ -3533,7 +3535,7 @@
         <v>351</v>
       </c>
       <c r="I353">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="354" spans="8:9">
@@ -3541,7 +3543,7 @@
         <v>352</v>
       </c>
       <c r="I354">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="355" spans="8:9">
@@ -3549,7 +3551,7 @@
         <v>353</v>
       </c>
       <c r="I355">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="356" spans="8:9">
@@ -3557,7 +3559,7 @@
         <v>354</v>
       </c>
       <c r="I356">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="357" spans="8:9">
@@ -3573,7 +3575,7 @@
         <v>356</v>
       </c>
       <c r="I358">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="359" spans="8:9">
@@ -3589,7 +3591,7 @@
         <v>358</v>
       </c>
       <c r="I360">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="361" spans="8:9">
@@ -3597,7 +3599,7 @@
         <v>359</v>
       </c>
       <c r="I361">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="362" spans="8:9">
@@ -3605,7 +3607,7 @@
         <v>360</v>
       </c>
       <c r="I362">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="363" spans="8:9">
@@ -3613,7 +3615,7 @@
         <v>361</v>
       </c>
       <c r="I363">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="364" spans="8:9">
@@ -3645,7 +3647,7 @@
         <v>365</v>
       </c>
       <c r="I367">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="368" spans="8:9">
@@ -3653,7 +3655,7 @@
         <v>366</v>
       </c>
       <c r="I368">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="369" spans="8:9">
@@ -3661,7 +3663,7 @@
         <v>367</v>
       </c>
       <c r="I369">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="370" spans="8:9">
@@ -3677,7 +3679,7 @@
         <v>369</v>
       </c>
       <c r="I371">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="372" spans="8:9">
@@ -3685,7 +3687,7 @@
         <v>370</v>
       </c>
       <c r="I372">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="373" spans="8:9">
@@ -3701,7 +3703,7 @@
         <v>372</v>
       </c>
       <c r="I374">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="375" spans="8:9">
@@ -3709,7 +3711,7 @@
         <v>373</v>
       </c>
       <c r="I375">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="376" spans="8:9">
@@ -3741,7 +3743,7 @@
         <v>377</v>
       </c>
       <c r="I379">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="380" spans="8:9">
@@ -3757,7 +3759,7 @@
         <v>379</v>
       </c>
       <c r="I381">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="382" spans="8:9">
@@ -3773,7 +3775,7 @@
         <v>381</v>
       </c>
       <c r="I383">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="384" spans="8:9">
@@ -3781,7 +3783,7 @@
         <v>382</v>
       </c>
       <c r="I384">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="385" spans="8:9">
@@ -3797,7 +3799,7 @@
         <v>384</v>
       </c>
       <c r="I386">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="387" spans="8:9">
@@ -3813,7 +3815,7 @@
         <v>386</v>
       </c>
       <c r="I388">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="389" spans="8:9">
@@ -3829,7 +3831,7 @@
         <v>388</v>
       </c>
       <c r="I390">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="391" spans="8:9">
@@ -3845,7 +3847,7 @@
         <v>390</v>
       </c>
       <c r="I392">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="393" spans="8:9">
@@ -3893,7 +3895,7 @@
         <v>396</v>
       </c>
       <c r="I398">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="399" spans="8:9">
@@ -3909,7 +3911,7 @@
         <v>398</v>
       </c>
       <c r="I400">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="401" spans="8:9">
@@ -3917,7 +3919,7 @@
         <v>399</v>
       </c>
       <c r="I401">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="402" spans="8:9">
@@ -3925,7 +3927,7 @@
         <v>400</v>
       </c>
       <c r="I402">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="403" spans="8:9">
@@ -3933,7 +3935,7 @@
         <v>401</v>
       </c>
       <c r="I403">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="404" spans="8:9">
@@ -3949,7 +3951,7 @@
         <v>403</v>
       </c>
       <c r="I405">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="406" spans="8:9">
@@ -3957,7 +3959,7 @@
         <v>404</v>
       </c>
       <c r="I406">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="407" spans="8:9">
@@ -3965,7 +3967,7 @@
         <v>405</v>
       </c>
       <c r="I407">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="408" spans="8:9">
@@ -3973,7 +3975,7 @@
         <v>406</v>
       </c>
       <c r="I408">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="409" spans="8:9">
@@ -4005,7 +4007,7 @@
         <v>410</v>
       </c>
       <c r="I412">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="413" spans="8:9">
@@ -4021,7 +4023,7 @@
         <v>412</v>
       </c>
       <c r="I414">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="415" spans="8:9">
@@ -4029,7 +4031,7 @@
         <v>413</v>
       </c>
       <c r="I415">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="416" spans="8:9">
@@ -4037,7 +4039,7 @@
         <v>414</v>
       </c>
       <c r="I416">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="417" spans="8:9">
@@ -4045,7 +4047,7 @@
         <v>415</v>
       </c>
       <c r="I417">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="418" spans="8:9">
@@ -4069,7 +4071,7 @@
         <v>418</v>
       </c>
       <c r="I420">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="421" spans="8:9">
@@ -4093,7 +4095,7 @@
         <v>421</v>
       </c>
       <c r="I423">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="424" spans="8:9">
@@ -4101,7 +4103,7 @@
         <v>422</v>
       </c>
       <c r="I424">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="425" spans="8:9">
@@ -4117,7 +4119,7 @@
         <v>424</v>
       </c>
       <c r="I426">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="427" spans="8:9">
@@ -4157,7 +4159,7 @@
         <v>429</v>
       </c>
       <c r="I431">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="432" spans="8:9">
@@ -4173,7 +4175,7 @@
         <v>431</v>
       </c>
       <c r="I433">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="434" spans="8:9">
@@ -4181,7 +4183,7 @@
         <v>432</v>
       </c>
       <c r="I434">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="435" spans="8:9">
@@ -4189,7 +4191,7 @@
         <v>433</v>
       </c>
       <c r="I435">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="436" spans="8:9">
@@ -4197,7 +4199,7 @@
         <v>434</v>
       </c>
       <c r="I436">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="437" spans="8:9">
@@ -4205,7 +4207,7 @@
         <v>435</v>
       </c>
       <c r="I437">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="438" spans="8:9">
@@ -4213,7 +4215,7 @@
         <v>436</v>
       </c>
       <c r="I438">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="439" spans="8:9">
@@ -4237,7 +4239,7 @@
         <v>439</v>
       </c>
       <c r="I441">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="442" spans="8:9">
@@ -4253,7 +4255,7 @@
         <v>441</v>
       </c>
       <c r="I443">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="444" spans="8:9">
@@ -4261,7 +4263,7 @@
         <v>442</v>
       </c>
       <c r="I444">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="445" spans="8:9">
@@ -4285,7 +4287,7 @@
         <v>445</v>
       </c>
       <c r="I447">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="448" spans="8:9">
@@ -4301,7 +4303,7 @@
         <v>447</v>
       </c>
       <c r="I449">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="450" spans="8:9">
@@ -4317,7 +4319,7 @@
         <v>449</v>
       </c>
       <c r="I451">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="452" spans="8:9">
@@ -4325,7 +4327,7 @@
         <v>450</v>
       </c>
       <c r="I452">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="453" spans="8:9">
@@ -4349,7 +4351,7 @@
         <v>453</v>
       </c>
       <c r="I455">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="456" spans="8:9">
@@ -4357,7 +4359,7 @@
         <v>454</v>
       </c>
       <c r="I456">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="457" spans="8:9">
@@ -4373,7 +4375,7 @@
         <v>456</v>
       </c>
       <c r="I458">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="459" spans="8:9">
@@ -4381,7 +4383,7 @@
         <v>457</v>
       </c>
       <c r="I459">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="460" spans="8:9">
@@ -4389,7 +4391,7 @@
         <v>458</v>
       </c>
       <c r="I460">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="461" spans="8:9">
@@ -4397,7 +4399,7 @@
         <v>459</v>
       </c>
       <c r="I461">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="462" spans="8:9">
@@ -4429,7 +4431,7 @@
         <v>463</v>
       </c>
       <c r="I465">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="466" spans="8:9">
@@ -4445,7 +4447,7 @@
         <v>465</v>
       </c>
       <c r="I467">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="468" spans="8:9">
@@ -4469,7 +4471,7 @@
         <v>468</v>
       </c>
       <c r="I470">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="471" spans="8:9">
@@ -4477,7 +4479,7 @@
         <v>469</v>
       </c>
       <c r="I471">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="472" spans="8:9">
@@ -4493,7 +4495,7 @@
         <v>471</v>
       </c>
       <c r="I473">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="474" spans="8:9">
@@ -4509,7 +4511,7 @@
         <v>473</v>
       </c>
       <c r="I475">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="476" spans="8:9">
@@ -4525,7 +4527,7 @@
         <v>475</v>
       </c>
       <c r="I477">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="478" spans="8:9">
@@ -4533,7 +4535,7 @@
         <v>476</v>
       </c>
       <c r="I478">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="479" spans="8:9">
@@ -4541,7 +4543,7 @@
         <v>477</v>
       </c>
       <c r="I479">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="480" spans="8:9">
@@ -4557,7 +4559,7 @@
         <v>479</v>
       </c>
       <c r="I481">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="482" spans="8:9">
@@ -4565,7 +4567,7 @@
         <v>480</v>
       </c>
       <c r="I482">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="483" spans="8:9">
@@ -4573,7 +4575,7 @@
         <v>481</v>
       </c>
       <c r="I483">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="484" spans="8:9">
@@ -4589,7 +4591,7 @@
         <v>483</v>
       </c>
       <c r="I485">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="486" spans="8:9">
@@ -4597,7 +4599,7 @@
         <v>484</v>
       </c>
       <c r="I486">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="487" spans="8:9">
@@ -4605,7 +4607,7 @@
         <v>485</v>
       </c>
       <c r="I487">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="488" spans="8:9">
@@ -4613,7 +4615,7 @@
         <v>486</v>
       </c>
       <c r="I488">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="489" spans="8:9">
@@ -4629,7 +4631,7 @@
         <v>488</v>
       </c>
       <c r="I490">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="491" spans="8:9">
@@ -4637,7 +4639,7 @@
         <v>489</v>
       </c>
       <c r="I491">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="492" spans="8:9">
@@ -4645,7 +4647,7 @@
         <v>490</v>
       </c>
       <c r="I492">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="493" spans="8:9">
@@ -4677,7 +4679,7 @@
         <v>494</v>
       </c>
       <c r="I496">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="497" spans="8:9">
@@ -4685,7 +4687,7 @@
         <v>495</v>
       </c>
       <c r="I497">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="498" spans="8:9">
@@ -4693,7 +4695,7 @@
         <v>496</v>
       </c>
       <c r="I498">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="499" spans="8:9">
@@ -4725,7 +4727,7 @@
         <v>500</v>
       </c>
       <c r="I502">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="503" spans="8:9">
@@ -4749,7 +4751,7 @@
         <v>503</v>
       </c>
       <c r="I505">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="506" spans="8:9">
@@ -4773,7 +4775,7 @@
         <v>506</v>
       </c>
       <c r="I508">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="509" spans="8:9">
@@ -4789,7 +4791,7 @@
         <v>508</v>
       </c>
       <c r="I510">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="511" spans="8:9">
@@ -4813,7 +4815,7 @@
         <v>511</v>
       </c>
       <c r="I513">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="514" spans="8:9">
@@ -4821,7 +4823,7 @@
         <v>512</v>
       </c>
       <c r="I514">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="515" spans="8:9">
@@ -4837,7 +4839,7 @@
         <v>514</v>
       </c>
       <c r="I516">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="517" spans="8:9">
@@ -4845,7 +4847,7 @@
         <v>515</v>
       </c>
       <c r="I517">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="518" spans="8:9">
@@ -4853,7 +4855,7 @@
         <v>516</v>
       </c>
       <c r="I518">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="519" spans="8:9">
@@ -4861,7 +4863,7 @@
         <v>517</v>
       </c>
       <c r="I519">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="520" spans="8:9">
@@ -4877,7 +4879,7 @@
         <v>519</v>
       </c>
       <c r="I521">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="522" spans="8:9">
@@ -4893,7 +4895,7 @@
         <v>521</v>
       </c>
       <c r="I523">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="524" spans="8:9">
@@ -4909,7 +4911,7 @@
         <v>523</v>
       </c>
       <c r="I525">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="526" spans="8:9">
@@ -4925,7 +4927,7 @@
         <v>525</v>
       </c>
       <c r="I527">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="528" spans="8:9">
@@ -4933,7 +4935,7 @@
         <v>526</v>
       </c>
       <c r="I528">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="529" spans="8:9">
@@ -4941,7 +4943,7 @@
         <v>527</v>
       </c>
       <c r="I529">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="530" spans="8:9">
@@ -4949,7 +4951,7 @@
         <v>528</v>
       </c>
       <c r="I530">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="531" spans="8:9">
@@ -4957,7 +4959,7 @@
         <v>529</v>
       </c>
       <c r="I531">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="532" spans="8:9">
@@ -5005,7 +5007,7 @@
         <v>535</v>
       </c>
       <c r="I537">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="538" spans="8:9">
@@ -5013,7 +5015,7 @@
         <v>536</v>
       </c>
       <c r="I538">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="539" spans="8:9">
@@ -5045,7 +5047,7 @@
         <v>540</v>
       </c>
       <c r="I542">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="543" spans="8:9">
@@ -5053,7 +5055,7 @@
         <v>541</v>
       </c>
       <c r="I543">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="544" spans="8:9">
@@ -5077,7 +5079,7 @@
         <v>544</v>
       </c>
       <c r="I546">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="547" spans="8:9">
@@ -5085,7 +5087,7 @@
         <v>545</v>
       </c>
       <c r="I547">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="548" spans="8:9">
@@ -5093,7 +5095,7 @@
         <v>546</v>
       </c>
       <c r="I548">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="549" spans="8:9">
@@ -5109,7 +5111,7 @@
         <v>548</v>
       </c>
       <c r="I550">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="551" spans="8:9">
@@ -5125,7 +5127,7 @@
         <v>550</v>
       </c>
       <c r="I552">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="553" spans="8:9">
@@ -5141,7 +5143,7 @@
         <v>552</v>
       </c>
       <c r="I554">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="555" spans="8:9">
@@ -5149,7 +5151,7 @@
         <v>553</v>
       </c>
       <c r="I555">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="556" spans="8:9">
@@ -5157,7 +5159,7 @@
         <v>554</v>
       </c>
       <c r="I556">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="557" spans="8:9">
@@ -5165,7 +5167,7 @@
         <v>555</v>
       </c>
       <c r="I557">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="558" spans="8:9">
@@ -5181,7 +5183,7 @@
         <v>557</v>
       </c>
       <c r="I559">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="560" spans="8:9">
@@ -5197,7 +5199,7 @@
         <v>559</v>
       </c>
       <c r="I561">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="562" spans="8:9">
@@ -5213,7 +5215,7 @@
         <v>561</v>
       </c>
       <c r="I563">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="564" spans="8:9">
@@ -5229,7 +5231,7 @@
         <v>563</v>
       </c>
       <c r="I565">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="566" spans="8:9">
@@ -5269,7 +5271,7 @@
         <v>568</v>
       </c>
       <c r="I570">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="571" spans="8:9">
@@ -5277,7 +5279,7 @@
         <v>569</v>
       </c>
       <c r="I571">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="572" spans="8:9">
@@ -5285,7 +5287,7 @@
         <v>570</v>
       </c>
       <c r="I572">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="573" spans="8:9">
@@ -5309,7 +5311,7 @@
         <v>573</v>
       </c>
       <c r="I575">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="576" spans="8:9">
@@ -5317,7 +5319,7 @@
         <v>574</v>
       </c>
       <c r="I576">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="577" spans="8:9">
@@ -5333,7 +5335,7 @@
         <v>576</v>
       </c>
       <c r="I578">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="579" spans="8:9">
@@ -5357,7 +5359,7 @@
         <v>579</v>
       </c>
       <c r="I581">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="582" spans="8:9">
@@ -5365,7 +5367,7 @@
         <v>580</v>
       </c>
       <c r="I582">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="583" spans="8:9">
@@ -5373,7 +5375,7 @@
         <v>581</v>
       </c>
       <c r="I583">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="584" spans="8:9">
@@ -5381,7 +5383,7 @@
         <v>582</v>
       </c>
       <c r="I584">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="585" spans="8:9">
@@ -5413,7 +5415,7 @@
         <v>586</v>
       </c>
       <c r="I588">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="589" spans="8:9">
@@ -5421,7 +5423,7 @@
         <v>587</v>
       </c>
       <c r="I589">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="590" spans="8:9">
@@ -5437,7 +5439,7 @@
         <v>589</v>
       </c>
       <c r="I591">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="592" spans="8:9">
@@ -5453,7 +5455,7 @@
         <v>591</v>
       </c>
       <c r="I593">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="594" spans="8:9">
@@ -5461,7 +5463,7 @@
         <v>592</v>
       </c>
       <c r="I594">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="595" spans="8:9">
@@ -5469,7 +5471,7 @@
         <v>593</v>
       </c>
       <c r="I595">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="596" spans="8:9">
@@ -5477,7 +5479,7 @@
         <v>594</v>
       </c>
       <c r="I596">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="597" spans="8:9">
@@ -5493,7 +5495,7 @@
         <v>596</v>
       </c>
       <c r="I598">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="599" spans="8:9">
@@ -5501,7 +5503,7 @@
         <v>597</v>
       </c>
       <c r="I599">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="600" spans="8:9">
@@ -5525,7 +5527,7 @@
         <v>600</v>
       </c>
       <c r="I602">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="603" spans="8:9">
@@ -5541,7 +5543,7 @@
         <v>602</v>
       </c>
       <c r="I604">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="605" spans="8:9">
@@ -5557,7 +5559,7 @@
         <v>604</v>
       </c>
       <c r="I606">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="607" spans="8:9">
@@ -5589,7 +5591,7 @@
         <v>608</v>
       </c>
       <c r="I610">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="611" spans="8:9">
@@ -5605,7 +5607,7 @@
         <v>610</v>
       </c>
       <c r="I612">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="613" spans="8:9">
@@ -5613,7 +5615,7 @@
         <v>611</v>
       </c>
       <c r="I613">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="614" spans="8:9">
@@ -5621,7 +5623,7 @@
         <v>612</v>
       </c>
       <c r="I614">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="615" spans="8:9">
@@ -5629,7 +5631,7 @@
         <v>613</v>
       </c>
       <c r="I615">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="616" spans="8:9">
@@ -5637,7 +5639,7 @@
         <v>614</v>
       </c>
       <c r="I616">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="617" spans="8:9">
@@ -5653,7 +5655,7 @@
         <v>616</v>
       </c>
       <c r="I618">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="619" spans="8:9">
@@ -5669,7 +5671,7 @@
         <v>618</v>
       </c>
       <c r="I620">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="621" spans="8:9">
@@ -5693,7 +5695,7 @@
         <v>621</v>
       </c>
       <c r="I623">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="624" spans="8:9">
@@ -5717,7 +5719,7 @@
         <v>624</v>
       </c>
       <c r="I626">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="627" spans="8:9">
@@ -5733,7 +5735,7 @@
         <v>626</v>
       </c>
       <c r="I628">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="629" spans="8:9">
@@ -5741,7 +5743,7 @@
         <v>627</v>
       </c>
       <c r="I629">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="630" spans="8:9">
@@ -5765,7 +5767,7 @@
         <v>630</v>
       </c>
       <c r="I632">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="633" spans="8:9">
@@ -5773,7 +5775,7 @@
         <v>631</v>
       </c>
       <c r="I633">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="634" spans="8:9">
@@ -5781,7 +5783,7 @@
         <v>632</v>
       </c>
       <c r="I634">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="635" spans="8:9">
@@ -5797,7 +5799,7 @@
         <v>634</v>
       </c>
       <c r="I636">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="637" spans="8:9">
@@ -5805,7 +5807,7 @@
         <v>635</v>
       </c>
       <c r="I637">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="638" spans="8:9">
@@ -5821,7 +5823,7 @@
         <v>637</v>
       </c>
       <c r="I639">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="640" spans="8:9">
@@ -5829,7 +5831,7 @@
         <v>638</v>
       </c>
       <c r="I640">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="641" spans="8:9">
@@ -5869,7 +5871,7 @@
         <v>643</v>
       </c>
       <c r="I645">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="646" spans="8:9">
@@ -5909,7 +5911,7 @@
         <v>648</v>
       </c>
       <c r="I650">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="651" spans="8:9">
@@ -5917,7 +5919,7 @@
         <v>649</v>
       </c>
       <c r="I651">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="652" spans="8:9">
@@ -5925,7 +5927,7 @@
         <v>650</v>
       </c>
       <c r="I652">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="653" spans="8:9">
@@ -5933,7 +5935,7 @@
         <v>651</v>
       </c>
       <c r="I653">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="654" spans="8:9">
@@ -5949,7 +5951,7 @@
         <v>653</v>
       </c>
       <c r="I655">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="656" spans="8:9">
@@ -5973,7 +5975,7 @@
         <v>656</v>
       </c>
       <c r="I658">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="659" spans="8:9">
@@ -5997,7 +5999,7 @@
         <v>659</v>
       </c>
       <c r="I661">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="662" spans="8:9">
@@ -6029,7 +6031,7 @@
         <v>663</v>
       </c>
       <c r="I665">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="666" spans="8:9">
@@ -6037,7 +6039,7 @@
         <v>664</v>
       </c>
       <c r="I666">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="667" spans="8:9">
@@ -6045,7 +6047,7 @@
         <v>665</v>
       </c>
       <c r="I667">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="668" spans="8:9">
@@ -6061,7 +6063,7 @@
         <v>667</v>
       </c>
       <c r="I669">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="670" spans="8:9">
@@ -6085,7 +6087,7 @@
         <v>670</v>
       </c>
       <c r="I672">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="673" spans="8:9">
@@ -6109,7 +6111,7 @@
         <v>673</v>
       </c>
       <c r="I675">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="676" spans="8:9">
@@ -6125,7 +6127,7 @@
         <v>675</v>
       </c>
       <c r="I677">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="678" spans="8:9">
@@ -6149,7 +6151,7 @@
         <v>678</v>
       </c>
       <c r="I680">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="681" spans="8:9">
@@ -6157,7 +6159,7 @@
         <v>679</v>
       </c>
       <c r="I681">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="682" spans="8:9">
@@ -6165,7 +6167,7 @@
         <v>680</v>
       </c>
       <c r="I682">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="683" spans="8:9">
@@ -6181,7 +6183,7 @@
         <v>682</v>
       </c>
       <c r="I684">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="685" spans="8:9">
@@ -6189,7 +6191,7 @@
         <v>683</v>
       </c>
       <c r="I685">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="686" spans="8:9">
@@ -6197,7 +6199,7 @@
         <v>684</v>
       </c>
       <c r="I686">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="687" spans="8:9">
@@ -6205,7 +6207,7 @@
         <v>685</v>
       </c>
       <c r="I687">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="688" spans="8:9">
@@ -6213,7 +6215,7 @@
         <v>686</v>
       </c>
       <c r="I688">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="689" spans="8:9">
@@ -6245,7 +6247,7 @@
         <v>690</v>
       </c>
       <c r="I692">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="693" spans="8:9">
@@ -6261,7 +6263,7 @@
         <v>692</v>
       </c>
       <c r="I694">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="695" spans="8:9">
@@ -6269,7 +6271,7 @@
         <v>693</v>
       </c>
       <c r="I695">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="696" spans="8:9">
@@ -6277,7 +6279,7 @@
         <v>694</v>
       </c>
       <c r="I696">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="697" spans="8:9">
@@ -6285,7 +6287,7 @@
         <v>695</v>
       </c>
       <c r="I697">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="698" spans="8:9">
@@ -6293,7 +6295,7 @@
         <v>696</v>
       </c>
       <c r="I698">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="699" spans="8:9">
@@ -6309,7 +6311,7 @@
         <v>698</v>
       </c>
       <c r="I700">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="701" spans="8:9">
@@ -6333,7 +6335,7 @@
         <v>701</v>
       </c>
       <c r="I703">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="704" spans="8:9">
@@ -6373,7 +6375,7 @@
         <v>706</v>
       </c>
       <c r="I708">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="709" spans="8:9">
@@ -6381,7 +6383,7 @@
         <v>707</v>
       </c>
       <c r="I709">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="710" spans="8:9">
@@ -6397,7 +6399,7 @@
         <v>709</v>
       </c>
       <c r="I711">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="712" spans="8:9">
@@ -6421,7 +6423,7 @@
         <v>712</v>
       </c>
       <c r="I714">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="715" spans="8:9">
@@ -6429,7 +6431,7 @@
         <v>713</v>
       </c>
       <c r="I715">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="716" spans="8:9">
@@ -6445,7 +6447,7 @@
         <v>715</v>
       </c>
       <c r="I717">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="718" spans="8:9">
@@ -6453,7 +6455,7 @@
         <v>716</v>
       </c>
       <c r="I718">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="719" spans="8:9">
@@ -6461,7 +6463,7 @@
         <v>717</v>
       </c>
       <c r="I719">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="720" spans="8:9">
@@ -6469,7 +6471,7 @@
         <v>718</v>
       </c>
       <c r="I720">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="721" spans="8:9">
@@ -6493,7 +6495,7 @@
         <v>721</v>
       </c>
       <c r="I723">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="724" spans="8:9">
@@ -6541,7 +6543,7 @@
         <v>727</v>
       </c>
       <c r="I729">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="730" spans="8:9">
@@ -6549,7 +6551,7 @@
         <v>728</v>
       </c>
       <c r="I730">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="731" spans="8:9">
@@ -6565,7 +6567,7 @@
         <v>730</v>
       </c>
       <c r="I732">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="733" spans="8:9">
@@ -6581,7 +6583,7 @@
         <v>732</v>
       </c>
       <c r="I734">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="735" spans="8:9">
@@ -6589,7 +6591,7 @@
         <v>733</v>
       </c>
       <c r="I735">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="736" spans="8:9">
@@ -6597,7 +6599,7 @@
         <v>734</v>
       </c>
       <c r="I736">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="737" spans="8:9">
@@ -6629,7 +6631,7 @@
         <v>738</v>
       </c>
       <c r="I740">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="741" spans="8:9">
@@ -6637,7 +6639,7 @@
         <v>739</v>
       </c>
       <c r="I741">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="742" spans="8:9">
@@ -6645,7 +6647,7 @@
         <v>740</v>
       </c>
       <c r="I742">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="743" spans="8:9">
@@ -6693,7 +6695,7 @@
         <v>746</v>
       </c>
       <c r="I748">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="749" spans="8:9">
@@ -6701,7 +6703,7 @@
         <v>747</v>
       </c>
       <c r="I749">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="750" spans="8:9">
@@ -6709,7 +6711,7 @@
         <v>748</v>
       </c>
       <c r="I750">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="751" spans="8:9">
@@ -6733,7 +6735,7 @@
         <v>751</v>
       </c>
       <c r="I753">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="754" spans="8:9">
@@ -6741,7 +6743,7 @@
         <v>752</v>
       </c>
       <c r="I754">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="755" spans="8:9">
@@ -6749,7 +6751,7 @@
         <v>753</v>
       </c>
       <c r="I755">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="756" spans="8:9">
@@ -6757,7 +6759,7 @@
         <v>754</v>
       </c>
       <c r="I756">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="757" spans="8:9">
@@ -6781,7 +6783,7 @@
         <v>757</v>
       </c>
       <c r="I759">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="760" spans="8:9">
@@ -6789,7 +6791,7 @@
         <v>758</v>
       </c>
       <c r="I760">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="761" spans="8:9">
@@ -6797,7 +6799,7 @@
         <v>759</v>
       </c>
       <c r="I761">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="762" spans="8:9">
@@ -6805,7 +6807,7 @@
         <v>760</v>
       </c>
       <c r="I762">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="763" spans="8:9">
@@ -6837,7 +6839,7 @@
         <v>764</v>
       </c>
       <c r="I766">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="767" spans="8:9">
@@ -6845,7 +6847,7 @@
         <v>765</v>
       </c>
       <c r="I767">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="768" spans="8:9">
@@ -6853,7 +6855,7 @@
         <v>766</v>
       </c>
       <c r="I768">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="769" spans="8:9">
@@ -6861,7 +6863,7 @@
         <v>767</v>
       </c>
       <c r="I769">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="770" spans="8:9">
@@ -6877,7 +6879,7 @@
         <v>769</v>
       </c>
       <c r="I771">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="772" spans="8:9">
@@ -6893,7 +6895,7 @@
         <v>771</v>
       </c>
       <c r="I773">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="774" spans="8:9">
@@ -6901,7 +6903,7 @@
         <v>772</v>
       </c>
       <c r="I774">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="775" spans="8:9">
@@ -6917,7 +6919,7 @@
         <v>774</v>
       </c>
       <c r="I776">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="777" spans="8:9">
@@ -6925,7 +6927,7 @@
         <v>775</v>
       </c>
       <c r="I777">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="778" spans="8:9">
@@ -6933,7 +6935,7 @@
         <v>776</v>
       </c>
       <c r="I778">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="779" spans="8:9">
@@ -6949,7 +6951,7 @@
         <v>778</v>
       </c>
       <c r="I780">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="781" spans="8:9">
@@ -6965,7 +6967,7 @@
         <v>780</v>
       </c>
       <c r="I782">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="783" spans="8:9">
@@ -6973,7 +6975,7 @@
         <v>781</v>
       </c>
       <c r="I783">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="784" spans="8:9">
@@ -6981,7 +6983,7 @@
         <v>782</v>
       </c>
       <c r="I784">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="785" spans="8:9">
@@ -6989,7 +6991,7 @@
         <v>783</v>
       </c>
       <c r="I785">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="786" spans="8:9">
@@ -7005,7 +7007,7 @@
         <v>785</v>
       </c>
       <c r="I787">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="788" spans="8:9">
@@ -7013,7 +7015,7 @@
         <v>786</v>
       </c>
       <c r="I788">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="789" spans="8:9">
@@ -7037,7 +7039,7 @@
         <v>789</v>
       </c>
       <c r="I791">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="792" spans="8:9">
@@ -7045,7 +7047,7 @@
         <v>790</v>
       </c>
       <c r="I792">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="793" spans="8:9">
@@ -7053,7 +7055,7 @@
         <v>791</v>
       </c>
       <c r="I793">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="794" spans="8:9">
@@ -7069,7 +7071,7 @@
         <v>793</v>
       </c>
       <c r="I795">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="796" spans="8:9">
@@ -7077,7 +7079,7 @@
         <v>794</v>
       </c>
       <c r="I796">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="797" spans="8:9">
@@ -7117,7 +7119,7 @@
         <v>799</v>
       </c>
       <c r="I801">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="802" spans="8:9">
@@ -7141,7 +7143,7 @@
         <v>802</v>
       </c>
       <c r="I804">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="805" spans="8:9">
@@ -7149,7 +7151,7 @@
         <v>803</v>
       </c>
       <c r="I805">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="806" spans="8:9">
@@ -7189,7 +7191,7 @@
         <v>808</v>
       </c>
       <c r="I810">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="811" spans="8:9">
@@ -7205,7 +7207,7 @@
         <v>810</v>
       </c>
       <c r="I812">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="813" spans="8:9">
@@ -7221,7 +7223,7 @@
         <v>812</v>
       </c>
       <c r="I814">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="815" spans="8:9">
@@ -7229,7 +7231,7 @@
         <v>813</v>
       </c>
       <c r="I815">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="816" spans="8:9">
@@ -7237,7 +7239,7 @@
         <v>814</v>
       </c>
       <c r="I816">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="817" spans="8:9">
@@ -7245,7 +7247,7 @@
         <v>815</v>
       </c>
       <c r="I817">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="818" spans="8:9">
@@ -7253,7 +7255,7 @@
         <v>816</v>
       </c>
       <c r="I818">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="819" spans="8:9">
@@ -7261,7 +7263,7 @@
         <v>817</v>
       </c>
       <c r="I819">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="820" spans="8:9">
@@ -7277,7 +7279,7 @@
         <v>819</v>
       </c>
       <c r="I821">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="822" spans="8:9">
@@ -7293,7 +7295,7 @@
         <v>821</v>
       </c>
       <c r="I823">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="824" spans="8:9">
@@ -7301,7 +7303,7 @@
         <v>822</v>
       </c>
       <c r="I824">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="825" spans="8:9">
@@ -7309,7 +7311,7 @@
         <v>823</v>
       </c>
       <c r="I825">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="826" spans="8:9">
@@ -7317,7 +7319,7 @@
         <v>824</v>
       </c>
       <c r="I826">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="827" spans="8:9">
@@ -7325,7 +7327,7 @@
         <v>825</v>
       </c>
       <c r="I827">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="828" spans="8:9">
@@ -7333,7 +7335,7 @@
         <v>826</v>
       </c>
       <c r="I828">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="829" spans="8:9">
@@ -7373,7 +7375,7 @@
         <v>831</v>
       </c>
       <c r="I833">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="834" spans="8:9">
@@ -7389,7 +7391,7 @@
         <v>833</v>
       </c>
       <c r="I835">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="836" spans="8:9">
@@ -7397,7 +7399,7 @@
         <v>834</v>
       </c>
       <c r="I836">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="837" spans="8:9">
@@ -7413,7 +7415,7 @@
         <v>836</v>
       </c>
       <c r="I838">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="839" spans="8:9">
@@ -7437,7 +7439,7 @@
         <v>839</v>
       </c>
       <c r="I841">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="842" spans="8:9">
@@ -7461,7 +7463,7 @@
         <v>842</v>
       </c>
       <c r="I844">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="845" spans="8:9">
@@ -7485,7 +7487,7 @@
         <v>845</v>
       </c>
       <c r="I847">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="848" spans="8:9">
@@ -7493,7 +7495,7 @@
         <v>846</v>
       </c>
       <c r="I848">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="849" spans="8:9">
@@ -7509,7 +7511,7 @@
         <v>848</v>
       </c>
       <c r="I850">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="851" spans="8:9">
@@ -7541,7 +7543,7 @@
         <v>852</v>
       </c>
       <c r="I854">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="855" spans="8:9">
@@ -7549,7 +7551,7 @@
         <v>853</v>
       </c>
       <c r="I855">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="856" spans="8:9">
@@ -7557,7 +7559,7 @@
         <v>854</v>
       </c>
       <c r="I856">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="857" spans="8:9">
@@ -7573,7 +7575,7 @@
         <v>856</v>
       </c>
       <c r="I858">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="859" spans="8:9">
@@ -7589,7 +7591,7 @@
         <v>858</v>
       </c>
       <c r="I860">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="861" spans="8:9">
@@ -7605,7 +7607,7 @@
         <v>860</v>
       </c>
       <c r="I862">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="863" spans="8:9">
@@ -7621,7 +7623,7 @@
         <v>862</v>
       </c>
       <c r="I864">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="865" spans="8:9">
@@ -7629,7 +7631,7 @@
         <v>863</v>
       </c>
       <c r="I865">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="866" spans="8:9">
@@ -7637,7 +7639,7 @@
         <v>864</v>
       </c>
       <c r="I866">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="867" spans="8:9">
@@ -7661,7 +7663,7 @@
         <v>867</v>
       </c>
       <c r="I869">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="870" spans="8:9">
@@ -7669,7 +7671,7 @@
         <v>868</v>
       </c>
       <c r="I870">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="871" spans="8:9">
@@ -7677,7 +7679,7 @@
         <v>869</v>
       </c>
       <c r="I871">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="872" spans="8:9">
@@ -7693,7 +7695,7 @@
         <v>871</v>
       </c>
       <c r="I873">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="874" spans="8:9">
@@ -7701,7 +7703,7 @@
         <v>872</v>
       </c>
       <c r="I874">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="875" spans="8:9">
@@ -7717,7 +7719,7 @@
         <v>874</v>
       </c>
       <c r="I876">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="877" spans="8:9">
@@ -7725,7 +7727,7 @@
         <v>875</v>
       </c>
       <c r="I877">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="878" spans="8:9">
@@ -7781,7 +7783,7 @@
         <v>882</v>
       </c>
       <c r="I884">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="885" spans="8:9">
@@ -7789,7 +7791,7 @@
         <v>883</v>
       </c>
       <c r="I885">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="886" spans="8:9">
@@ -7821,7 +7823,7 @@
         <v>887</v>
       </c>
       <c r="I889">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="890" spans="8:9">
@@ -7829,7 +7831,7 @@
         <v>888</v>
       </c>
       <c r="I890">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="891" spans="8:9">
@@ -7861,7 +7863,7 @@
         <v>892</v>
       </c>
       <c r="I894">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="895" spans="8:9">
@@ -7869,7 +7871,7 @@
         <v>893</v>
       </c>
       <c r="I895">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="896" spans="8:9">
@@ -7893,7 +7895,7 @@
         <v>896</v>
       </c>
       <c r="I898">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="899" spans="8:9">
@@ -7901,7 +7903,7 @@
         <v>897</v>
       </c>
       <c r="I899">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="900" spans="8:9">
@@ -7909,7 +7911,7 @@
         <v>898</v>
       </c>
       <c r="I900">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="901" spans="8:9">
@@ -7917,7 +7919,7 @@
         <v>899</v>
       </c>
       <c r="I901">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="902" spans="8:9">
@@ -7997,7 +7999,7 @@
         <v>909</v>
       </c>
       <c r="I911">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="912" spans="8:9">
@@ -8013,7 +8015,7 @@
         <v>911</v>
       </c>
       <c r="I913">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="914" spans="8:9">
@@ -8029,7 +8031,7 @@
         <v>913</v>
       </c>
       <c r="I915">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="916" spans="8:9">
@@ -8053,7 +8055,7 @@
         <v>916</v>
       </c>
       <c r="I918">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="919" spans="8:9">
@@ -8061,7 +8063,7 @@
         <v>917</v>
       </c>
       <c r="I919">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="920" spans="8:9">
@@ -8077,7 +8079,7 @@
         <v>919</v>
       </c>
       <c r="I921">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="922" spans="8:9">
@@ -8125,7 +8127,7 @@
         <v>925</v>
       </c>
       <c r="I927">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="928" spans="8:9">
@@ -8149,7 +8151,7 @@
         <v>928</v>
       </c>
       <c r="I930">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="931" spans="8:9">
@@ -8157,7 +8159,7 @@
         <v>929</v>
       </c>
       <c r="I931">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="932" spans="8:9">
@@ -8189,7 +8191,7 @@
         <v>933</v>
       </c>
       <c r="I935">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="936" spans="8:9">
@@ -8205,7 +8207,7 @@
         <v>935</v>
       </c>
       <c r="I937">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="938" spans="8:9">
@@ -8213,7 +8215,7 @@
         <v>936</v>
       </c>
       <c r="I938">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="939" spans="8:9">
@@ -8237,7 +8239,7 @@
         <v>939</v>
       </c>
       <c r="I941">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="942" spans="8:9">
@@ -8253,7 +8255,7 @@
         <v>941</v>
       </c>
       <c r="I943">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="944" spans="8:9">
@@ -8269,7 +8271,7 @@
         <v>943</v>
       </c>
       <c r="I945">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="946" spans="8:9">
@@ -8277,7 +8279,7 @@
         <v>944</v>
       </c>
       <c r="I946">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="947" spans="8:9">
@@ -8293,7 +8295,7 @@
         <v>946</v>
       </c>
       <c r="I948">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="949" spans="8:9">
@@ -8309,7 +8311,7 @@
         <v>948</v>
       </c>
       <c r="I950">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="951" spans="8:9">
@@ -8325,7 +8327,7 @@
         <v>950</v>
       </c>
       <c r="I952">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="953" spans="8:9">
@@ -8333,7 +8335,7 @@
         <v>951</v>
       </c>
       <c r="I953">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="954" spans="8:9">
@@ -8365,7 +8367,7 @@
         <v>955</v>
       </c>
       <c r="I957">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="958" spans="8:9">
@@ -8373,7 +8375,7 @@
         <v>956</v>
       </c>
       <c r="I958">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="959" spans="8:9">
@@ -8389,7 +8391,7 @@
         <v>958</v>
       </c>
       <c r="I960">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="961" spans="8:9">
@@ -8397,7 +8399,7 @@
         <v>959</v>
       </c>
       <c r="I961">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="962" spans="8:9">
@@ -8429,7 +8431,7 @@
         <v>963</v>
       </c>
       <c r="I965">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="966" spans="8:9">
@@ -8437,7 +8439,7 @@
         <v>964</v>
       </c>
       <c r="I966">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="967" spans="8:9">
@@ -8445,7 +8447,7 @@
         <v>965</v>
       </c>
       <c r="I967">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="968" spans="8:9">
@@ -8453,7 +8455,7 @@
         <v>966</v>
       </c>
       <c r="I968">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="969" spans="8:9">
@@ -8469,7 +8471,7 @@
         <v>968</v>
       </c>
       <c r="I970">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="971" spans="8:9">
@@ -8477,7 +8479,7 @@
         <v>969</v>
       </c>
       <c r="I971">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="972" spans="8:9">
@@ -8485,7 +8487,7 @@
         <v>970</v>
       </c>
       <c r="I972">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="973" spans="8:9">
@@ -8517,7 +8519,7 @@
         <v>974</v>
       </c>
       <c r="I976">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="977" spans="8:9">
@@ -8525,7 +8527,7 @@
         <v>975</v>
       </c>
       <c r="I977">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="978" spans="8:9">
@@ -8533,7 +8535,7 @@
         <v>976</v>
       </c>
       <c r="I978">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="979" spans="8:9">
@@ -8557,7 +8559,7 @@
         <v>979</v>
       </c>
       <c r="I981">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="982" spans="8:9">
@@ -8573,7 +8575,7 @@
         <v>981</v>
       </c>
       <c r="I983">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="984" spans="8:9">
@@ -8589,7 +8591,7 @@
         <v>983</v>
       </c>
       <c r="I985">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="986" spans="8:9">
@@ -8637,7 +8639,7 @@
         <v>989</v>
       </c>
       <c r="I991">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="992" spans="8:9">
@@ -8645,7 +8647,7 @@
         <v>990</v>
       </c>
       <c r="I992">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="993" spans="8:9">
@@ -8661,7 +8663,7 @@
         <v>992</v>
       </c>
       <c r="I994">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="995" spans="8:9">
@@ -8669,7 +8671,7 @@
         <v>993</v>
       </c>
       <c r="I995">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="996" spans="8:9">
@@ -8701,7 +8703,7 @@
         <v>997</v>
       </c>
       <c r="I999">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1000" spans="8:9">
@@ -8709,7 +8711,7 @@
         <v>998</v>
       </c>
       <c r="I1000">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1001" spans="8:9">
@@ -8717,7 +8719,7 @@
         <v>999</v>
       </c>
       <c r="I1001">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1002" spans="8:9">
@@ -8725,7 +8727,7 @@
         <v>1000</v>
       </c>
       <c r="I1002">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>